<commit_message>
Updated Drought Action Start Month
Changed drought action start month from June to July.
</commit_message>
<xml_diff>
--- a/misc/One_Drought_User_Interface_w_NOAA_Index.xlsx
+++ b/misc/One_Drought_User_Interface_w_NOAA_Index.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wtravis\Google Drive\Ranch-Drought\Ranch_Drought_Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ucbfiles.colorado.edu\erlb\Users\wtravis\Documents\GitHub\drought_decision_model\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14745" tabRatio="653" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14745" tabRatio="653" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="senseInfo" sheetId="12" state="hidden" r:id="rId1"/>
@@ -107,7 +107,7 @@
     <definedName name="RiskUseFixedSeed" hidden="1">FALSE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">TRUE</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1195,7 +1195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="13">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -3264,7 +3264,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3356,6 +3356,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9789-49F5-B99C-58455B98FCCE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3402,24 +3407,29 @@
                   <c:v>46867.366500000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55138.572309009673</c:v>
+                  <c:v>62597.842528418929</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31140.179757549762</c:v>
+                  <c:v>31204.142999681197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31407.20679897075</c:v>
+                  <c:v>31471.718525903463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31676.523597271924</c:v>
+                  <c:v>31741.588512263086</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31948.149787118531</c:v>
+                  <c:v>32013.77263375574</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9789-49F5-B99C-58455B98FCCE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3466,24 +3476,29 @@
                   <c:v>46867.366500000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-33275.741692702402</c:v>
+                  <c:v>-13475.741692702402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28504.443289974348</c:v>
+                  <c:v>29791.443289974348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29775.456416274305</c:v>
+                  <c:v>30754.381355052752</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30751.169868822304</c:v>
+                  <c:v>31018.100175172331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31014.861150447457</c:v>
+                  <c:v>31284.080384174435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9789-49F5-B99C-58455B98FCCE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -3530,24 +3545,29 @@
                   <c:v>46867.366500000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-28116.821692702419</c:v>
+                  <c:v>-17358.679192702402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28839.773089974347</c:v>
+                  <c:v>29539.052352474348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30125.738572056303</c:v>
+                  <c:v>30703.680384013693</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30821.535491343137</c:v>
+                  <c:v>30966.96444330661</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30821.535491343137</c:v>
+                  <c:v>30966.96444330661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9789-49F5-B99C-58455B98FCCE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -3612,6 +3632,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9789-49F5-B99C-58455B98FCCE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -3676,6 +3701,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-9789-49F5-B99C-58455B98FCCE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3769,6 +3799,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
@@ -3814,7 +3845,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3896,6 +3927,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EFDE-4C3E-BC22-32B29CF6C3AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3942,24 +3978,29 @@
                   <c:v>514687.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>547825.06060398067</c:v>
+                  <c:v>552942.11997449538</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>569187.22391765972</c:v>
+                  <c:v>574348.1620722767</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>590732.56778175372</c:v>
+                  <c:v>595937.76098104648</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>612462.66296948225</c:v>
+                  <c:v>617712.49070045887</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>634379.09372344555</c:v>
+                  <c:v>639673.9387272154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EFDE-4C3E-BC22-32B29CF6C3AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4006,24 +4047,29 @@
                   <c:v>514687.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>476724.2583072976</c:v>
+                  <c:v>496524.2583072976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>496278.30640422</c:v>
+                  <c:v>516961.18840421998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>516704.26950578415</c:v>
+                  <c:v>538058.69401378615</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>537799.57203579624</c:v>
+                  <c:v>559337.11073395447</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>559075.76678500324</c:v>
+                  <c:v>580797.98987749801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EFDE-4C3E-BC22-32B29CF6C3AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -4070,24 +4116,29 @@
                   <c:v>514687.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>481883.17830729758</c:v>
+                  <c:v>492641.3208072976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>501667.26264701999</c:v>
+                  <c:v>512905.110721095</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>522333.51930745062</c:v>
+                  <c:v>533967.83546452841</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>543477.09265451203</c:v>
+                  <c:v>555211.17307263671</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>564801.97214302444</c:v>
+                  <c:v>576636.67230073456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EFDE-4C3E-BC22-32B29CF6C3AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -4152,6 +4203,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-EFDE-4C3E-BC22-32B29CF6C3AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -4216,6 +4272,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EFDE-4C3E-BC22-32B29CF6C3AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4356,7 +4417,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4474,6 +4535,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-845E-4902-B526-06FF0A5A4F77}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -4529,24 +4595,29 @@
                   <c:v>514687.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>547825.06060398067</c:v>
+                  <c:v>552942.11997449538</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>569187.22391765972</c:v>
+                  <c:v>574348.1620722767</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>590732.56778175372</c:v>
+                  <c:v>595937.76098104648</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>612462.66296948225</c:v>
+                  <c:v>617712.49070045887</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>634379.09372344555</c:v>
+                  <c:v>639673.9387272154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-845E-4902-B526-06FF0A5A4F77}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4602,24 +4673,29 @@
                   <c:v>514687.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>476724.2583072976</c:v>
+                  <c:v>496524.2583072976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>496278.30640422</c:v>
+                  <c:v>516961.18840421998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>516704.26950578415</c:v>
+                  <c:v>538058.69401378615</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>537799.57203579624</c:v>
+                  <c:v>559337.11073395447</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>559075.76678500324</c:v>
+                  <c:v>580797.98987749801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-845E-4902-B526-06FF0A5A4F77}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4675,24 +4751,29 @@
                   <c:v>514687.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>481883.17830729758</c:v>
+                  <c:v>492641.3208072976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>501667.26264701999</c:v>
+                  <c:v>512905.110721095</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>522333.51930745062</c:v>
+                  <c:v>533967.83546452841</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>543477.09265451203</c:v>
+                  <c:v>555211.17307263671</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>564801.97214302444</c:v>
+                  <c:v>576636.67230073456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-845E-4902-B526-06FF0A5A4F77}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -4766,6 +4847,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-845E-4902-B526-06FF0A5A4F77}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -4839,6 +4925,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-845E-4902-B526-06FF0A5A4F77}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4960,7 +5051,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5079,6 +5170,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-99FE-41E1-95D2-A3D5A1653148}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5134,24 +5230,29 @@
                   <c:v>46867.366500000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55138.572309009673</c:v>
+                  <c:v>62597.842528418929</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31140.179757549762</c:v>
+                  <c:v>31204.142999681197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31407.20679897075</c:v>
+                  <c:v>31471.718525903463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31676.523597271924</c:v>
+                  <c:v>31741.588512263086</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31948.149787118531</c:v>
+                  <c:v>32013.77263375574</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-99FE-41E1-95D2-A3D5A1653148}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -5198,24 +5299,29 @@
                   <c:v>46867.366500000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-33275.741692702402</c:v>
+                  <c:v>-13475.741692702402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28504.443289974348</c:v>
+                  <c:v>29791.443289974348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29775.456416274305</c:v>
+                  <c:v>30754.381355052752</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30751.169868822304</c:v>
+                  <c:v>31018.100175172331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31014.861150447457</c:v>
+                  <c:v>31284.080384174435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-99FE-41E1-95D2-A3D5A1653148}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -5262,24 +5368,29 @@
                   <c:v>46867.366500000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-28116.821692702419</c:v>
+                  <c:v>-17358.679192702402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28839.773089974347</c:v>
+                  <c:v>29539.052352474348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30125.738572056303</c:v>
+                  <c:v>30703.680384013693</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30821.535491343137</c:v>
+                  <c:v>30966.96444330661</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31085.830158181405</c:v>
+                  <c:v>31232.506163407961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-99FE-41E1-95D2-A3D5A1653148}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -5353,6 +5464,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-99FE-41E1-95D2-A3D5A1653148}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -5426,6 +5542,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-99FE-41E1-95D2-A3D5A1653148}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6028,7 +6149,7 @@
     <row r="2" spans="1:85" x14ac:dyDescent="0.2">
       <c r="E2" s="148">
         <f>'Ranch Strategies'!$Q$149</f>
-        <v>634379.09372344555</v>
+        <v>639673.9387272154</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -6131,7 +6252,7 @@
       </c>
       <c r="E5" s="160">
         <f>'Ranch Strategies'!$I$13</f>
-        <v>0.77091180097417411</v>
+        <v>0.82714981978038837</v>
       </c>
       <c r="F5" t="s">
         <v>143</v>
@@ -6275,8 +6396,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B3:CK80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6401,11 +6522,11 @@
       <c r="L8" s="407"/>
       <c r="M8" s="418">
         <f>IF($G$51=1,'Ranch Strategies'!Q84,'Ranch Strategies'!Q167)</f>
-        <v>55138.572309009673</v>
+        <v>62597.842528418929</v>
       </c>
       <c r="N8" s="456">
         <f>IF($G$51=1,'Ranch Strategies'!Q167,'Ranch Strategies'!Q84)</f>
-        <v>23314.314001712075</v>
+        <v>30773.584221121331</v>
       </c>
     </row>
     <row r="9" spans="2:89" x14ac:dyDescent="0.2">
@@ -6416,7 +6537,7 @@
       <c r="D9" s="391"/>
       <c r="E9" s="391"/>
       <c r="F9" s="380">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G9" s="437"/>
       <c r="H9" s="442"/>
@@ -6427,11 +6548,11 @@
       <c r="L9" s="407"/>
       <c r="M9" s="418">
         <f>IF($G$51=1,'Ranch Strategies'!R84,'Ranch Strategies'!R167)</f>
-        <v>-33275.741692702402</v>
+        <v>-13475.741692702402</v>
       </c>
       <c r="N9" s="456">
         <f>IF($G$51=1,'Ranch Strategies'!R167,'Ranch Strategies'!R84)</f>
-        <v>-65100</v>
+        <v>-45300</v>
       </c>
       <c r="CJ9" s="363"/>
       <c r="CK9" s="357"/>
@@ -6444,7 +6565,7 @@
       <c r="D10" s="391"/>
       <c r="E10" s="391"/>
       <c r="F10" s="380">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G10" s="437"/>
       <c r="H10" s="442"/>
@@ -6455,11 +6576,11 @@
       <c r="L10" s="407"/>
       <c r="M10" s="418">
         <f>IF($G$51=1,'Ranch Strategies'!S84,'Ranch Strategies'!S167)</f>
-        <v>-28116.821692702419</v>
+        <v>-17358.679192702402</v>
       </c>
       <c r="N10" s="456">
         <f>IF($G$51=1,'Ranch Strategies'!S167,'Ranch Strategies'!S84)</f>
-        <v>-59941.080000000016</v>
+        <v>-49182.9375</v>
       </c>
       <c r="CJ10" s="363"/>
       <c r="CK10" s="357"/>
@@ -6643,11 +6764,11 @@
       <c r="L15" s="407"/>
       <c r="M15" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!Q99,'Ranch Strategies'!Q182)</f>
-        <v>31140.179757549762</v>
+        <v>31204.142999681197</v>
       </c>
       <c r="N15" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!Q182,'Ranch Strategies'!Q99)</f>
-        <v>37699.92024256468</v>
+        <v>37763.883484696118</v>
       </c>
       <c r="P15" s="149">
         <f>'Ranch Strategies'!E80</f>
@@ -6659,15 +6780,15 @@
       </c>
       <c r="R15" s="148">
         <f>'Ranch Strategies'!Q92</f>
-        <v>547825.06060398067</v>
+        <v>552942.11997449538</v>
       </c>
       <c r="S15" s="148">
         <f>'Ranch Strategies'!R92</f>
-        <v>476724.2583072976</v>
+        <v>496524.2583072976</v>
       </c>
       <c r="T15" s="148">
         <f>'Ranch Strategies'!S92</f>
-        <v>481883.17830729758</v>
+        <v>492641.3208072976</v>
       </c>
       <c r="U15" s="148">
         <f>'Ranch Strategies'!T92</f>
@@ -6702,11 +6823,11 @@
       <c r="L16" s="407"/>
       <c r="M16" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!R99,'Ranch Strategies'!R182)</f>
-        <v>28504.443289974348</v>
+        <v>29791.443289974348</v>
       </c>
       <c r="N16" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!R182,'Ranch Strategies'!R99)</f>
-        <v>33268.5</v>
+        <v>34555.5</v>
       </c>
       <c r="P16" s="149">
         <f>'Ranch Strategies'!E94</f>
@@ -6718,15 +6839,15 @@
       </c>
       <c r="R16" s="148">
         <f>'Ranch Strategies'!Q107</f>
-        <v>569187.22391765972</v>
+        <v>574348.1620722767</v>
       </c>
       <c r="S16" s="148">
         <f>'Ranch Strategies'!R107</f>
-        <v>496278.30640422</v>
+        <v>516961.18840421998</v>
       </c>
       <c r="T16" s="148">
         <f>'Ranch Strategies'!S107</f>
-        <v>501667.26264701999</v>
+        <v>512905.110721095</v>
       </c>
       <c r="U16" s="148">
         <f>'Ranch Strategies'!T107</f>
@@ -6755,11 +6876,11 @@
       <c r="L17" s="407"/>
       <c r="M17" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!S99,'Ranch Strategies'!S182)</f>
-        <v>28839.773089974347</v>
+        <v>29539.052352474348</v>
       </c>
       <c r="N17" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!S182,'Ranch Strategies'!S99)</f>
-        <v>33603.8298</v>
+        <v>34303.1090625</v>
       </c>
       <c r="P17" s="149">
         <f>'Ranch Strategies'!E109</f>
@@ -6771,15 +6892,15 @@
       </c>
       <c r="R17" s="148">
         <f>'Ranch Strategies'!Q121</f>
-        <v>590732.56778175372</v>
+        <v>595937.76098104648</v>
       </c>
       <c r="S17" s="148">
         <f>'Ranch Strategies'!R121</f>
-        <v>516704.26950578415</v>
+        <v>538058.69401378615</v>
       </c>
       <c r="T17" s="148">
         <f>'Ranch Strategies'!S121</f>
-        <v>522333.51930745062</v>
+        <v>533967.83546452841</v>
       </c>
       <c r="U17" s="148">
         <f>'Ranch Strategies'!T121</f>
@@ -6828,15 +6949,15 @@
       </c>
       <c r="R18" s="148">
         <f>'Ranch Strategies'!Q135</f>
-        <v>612462.66296948225</v>
+        <v>617712.49070045887</v>
       </c>
       <c r="S18" s="148">
         <f>'Ranch Strategies'!R135</f>
-        <v>537799.57203579624</v>
+        <v>559337.11073395447</v>
       </c>
       <c r="T18" s="148">
         <f>'Ranch Strategies'!S135</f>
-        <v>543477.09265451203</v>
+        <v>555211.17307263671</v>
       </c>
       <c r="U18" s="148">
         <f>'Ranch Strategies'!T135</f>
@@ -6885,15 +7006,15 @@
       </c>
       <c r="R19" s="148">
         <f>'Ranch Strategies'!Q149</f>
-        <v>634379.09372344555</v>
+        <v>639673.9387272154</v>
       </c>
       <c r="S19" s="148">
         <f>'Ranch Strategies'!R149</f>
-        <v>559075.76678500324</v>
+        <v>580797.98987749801</v>
       </c>
       <c r="T19" s="148">
         <f>'Ranch Strategies'!S149</f>
-        <v>564801.97214302444</v>
+        <v>576636.67230073456</v>
       </c>
       <c r="U19" s="148">
         <f>'Ranch Strategies'!T149</f>
@@ -6978,11 +7099,11 @@
       <c r="L22" s="407"/>
       <c r="M22" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!Q114,'Ranch Strategies'!Q197)</f>
-        <v>31407.20679897075</v>
+        <v>31471.718525903463</v>
       </c>
       <c r="N22" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!Q197,'Ranch Strategies'!Q114)</f>
-        <v>38023.19705864467</v>
+        <v>38087.708785577386</v>
       </c>
       <c r="CH22" s="468">
         <v>10</v>
@@ -7003,11 +7124,11 @@
       <c r="L23" s="407"/>
       <c r="M23" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!R114,'Ranch Strategies'!R197)</f>
-        <v>29775.456416274305</v>
+        <v>30754.381355052752</v>
       </c>
       <c r="N23" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!R197,'Ranch Strategies'!R114)</f>
-        <v>34751.942414999998</v>
+        <v>36096.329745000003</v>
       </c>
       <c r="CH23" s="468">
         <v>11</v>
@@ -7028,11 +7149,11 @@
       <c r="L24" s="407"/>
       <c r="M24" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!S114,'Ranch Strategies'!S197)</f>
-        <v>30125.738572056303</v>
+        <v>30703.680384013693</v>
       </c>
       <c r="N24" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!S197,'Ranch Strategies'!S114)</f>
-        <v>35102.224570781997</v>
+        <v>35832.684695596872</v>
       </c>
       <c r="CH24" s="468">
         <v>12</v>
@@ -7152,11 +7273,11 @@
       <c r="L29" s="407"/>
       <c r="M29" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!Q128,'Ranch Strategies'!Q211)</f>
-        <v>31676.523597271924</v>
+        <v>31741.588512263086</v>
       </c>
       <c r="N29" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!Q211,'Ranch Strategies'!Q128)</f>
-        <v>38349.245973422549</v>
+        <v>38414.310888413711</v>
       </c>
     </row>
     <row r="30" spans="2:86" x14ac:dyDescent="0.2">
@@ -7178,11 +7299,11 @@
       <c r="L30" s="407"/>
       <c r="M30" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!R128,'Ranch Strategies'!R211)</f>
-        <v>30751.169868822304</v>
+        <v>31018.100175172331</v>
       </c>
       <c r="N30" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!R211,'Ranch Strategies'!R128)</f>
-        <v>36301.531527284853</v>
+        <v>37539.589440063377</v>
       </c>
     </row>
     <row r="31" spans="2:86" x14ac:dyDescent="0.2">
@@ -7200,11 +7321,11 @@
       <c r="L31" s="407"/>
       <c r="M31" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!S128,'Ranch Strategies'!S211)</f>
-        <v>30821.535491343137</v>
+        <v>30966.96444330661</v>
       </c>
       <c r="N31" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!S211,'Ranch Strategies'!S128)</f>
-        <v>36667.432764393168</v>
+        <v>37430.464106173538</v>
       </c>
     </row>
     <row r="32" spans="2:86" x14ac:dyDescent="0.2">
@@ -7322,11 +7443,11 @@
       <c r="L36" s="407"/>
       <c r="M36" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!Q142,'Ranch Strategies'!Q225)</f>
-        <v>31948.149787118531</v>
+        <v>32013.77263375574</v>
       </c>
       <c r="N36" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!Q225, 'Ranch Strategies'!Q142)</f>
-        <v>38678.090757644648</v>
+        <v>38743.71360428186</v>
       </c>
       <c r="P36" s="403"/>
       <c r="Q36" s="432" t="s">
@@ -7356,11 +7477,11 @@
       <c r="L37" s="407"/>
       <c r="M37" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!R142,'Ranch Strategies'!R225)</f>
-        <v>31014.861150447457</v>
+        <v>31284.080384174435</v>
       </c>
       <c r="N37" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!R225, 'Ranch Strategies'!R142)</f>
-        <v>37580.810926555096</v>
+        <v>37861.49141951192</v>
       </c>
       <c r="P37" s="406"/>
       <c r="Q37" s="407"/>
@@ -7388,11 +7509,11 @@
       <c r="L38" s="407"/>
       <c r="M38" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!S142,'Ranch Strategies'!S225)</f>
-        <v>31085.830158181405</v>
+        <v>31232.506163407961</v>
       </c>
       <c r="N38" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!S225, 'Ranch Strategies'!S142)</f>
-        <v>37654.314152184124</v>
+        <v>37807.59394243612</v>
       </c>
       <c r="P38" s="406"/>
       <c r="Q38" s="407" t="s">
@@ -7449,16 +7570,16 @@
       </c>
       <c r="R39" s="457">
         <f>IF($G$51=1, 'Ranch Strategies'!Q152,'Ranch Strategies'!Q235)</f>
-        <v>119691.59372344555</v>
+        <v>124986.4387272154</v>
       </c>
       <c r="S39" s="458"/>
       <c r="T39" s="436">
         <f>IF($G$51=1, 'Ranch Strategies'!R152, 'Ranch Strategies'!R235)</f>
-        <v>44388.266785003245</v>
+        <v>66110.48987749801</v>
       </c>
       <c r="U39" s="436">
         <f>IF($G$51=1, 'Ranch Strategies'!S152, 'Ranch Strategies'!S235)</f>
-        <v>50114.472143024439</v>
+        <v>61949.172300734557</v>
       </c>
       <c r="V39" s="459">
         <f>IF($G$51=1, 'Ranch Strategies'!T152,'Ranch Strategies'!T235)</f>
@@ -7501,16 +7622,16 @@
       </c>
       <c r="R40" s="462">
         <f>IF($G$51=1, 'Ranch Strategies'!Q235,'Ranch Strategies'!Q152)</f>
-        <v>116092.93087131623</v>
+        <v>121387.77587508596</v>
       </c>
       <c r="S40" s="463"/>
       <c r="T40" s="464">
         <f>IF($G$51=1, 'Ranch Strategies'!R235,'Ranch Strategies'!R152)</f>
-        <v>27557.810420024209</v>
+        <v>50204.796674738638</v>
       </c>
       <c r="U40" s="464">
         <f>IF($G$51=1, 'Ranch Strategies'!S235,'Ranch Strategies'!S152)</f>
-        <v>33488.491683128406</v>
+        <v>45856.024839400663</v>
       </c>
       <c r="V40" s="462">
         <f>IF($G$51=1, 'Ranch Strategies'!T235,'Ranch Strategies'!T152)</f>
@@ -7666,11 +7787,11 @@
       <c r="L48" s="407"/>
       <c r="M48" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!Q92,'Ranch Strategies'!Q175)</f>
-        <v>547825.06060398067</v>
+        <v>552942.11997449538</v>
       </c>
       <c r="N48" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!Q175,'Ranch Strategies'!Q92)</f>
-        <v>525993.61940517451</v>
+        <v>531110.67877568922</v>
       </c>
     </row>
     <row r="49" spans="2:23" ht="15" x14ac:dyDescent="0.25">
@@ -7690,11 +7811,11 @@
       <c r="L49" s="407"/>
       <c r="M49" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!R92,'Ranch Strategies'!R175)</f>
-        <v>476724.2583072976</v>
+        <v>496524.2583072976</v>
       </c>
       <c r="N49" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!R175,'Ranch Strategies'!R92)</f>
-        <v>444900</v>
+        <v>464700</v>
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.2">
@@ -7712,11 +7833,11 @@
       <c r="L50" s="407"/>
       <c r="M50" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!S92,'Ranch Strategies'!S175)</f>
-        <v>481883.17830729758</v>
+        <v>492641.3208072976</v>
       </c>
       <c r="N50" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!S175,'Ranch Strategies'!S92)</f>
-        <v>450058.92</v>
+        <v>460817.0625</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.2">
@@ -7764,7 +7885,7 @@
       <c r="L52" s="407"/>
       <c r="M52" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!R92,'Ranch Strategies'!R175)</f>
-        <v>476724.2583072976</v>
+        <v>496524.2583072976</v>
       </c>
       <c r="N52" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!U175,'Ranch Strategies'!U92)</f>
@@ -7836,11 +7957,11 @@
       <c r="L55" s="407"/>
       <c r="M55" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!Q107,'Ranch Strategies'!Q190)</f>
-        <v>569187.22391765972</v>
+        <v>574348.1620722767</v>
       </c>
       <c r="N55" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!Q190,'Ranch Strategies'!Q107)</f>
-        <v>551855.7646915738</v>
+        <v>557016.70284619078</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.2">
@@ -7858,11 +7979,11 @@
       <c r="L56" s="407"/>
       <c r="M56" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!R107,'Ranch Strategies'!R190)</f>
-        <v>496278.30640422</v>
+        <v>516961.18840421998</v>
       </c>
       <c r="N56" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!R190,'Ranch Strategies'!R107)</f>
-        <v>467722.19099999999</v>
+        <v>488405.07299999997</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.2">
@@ -7880,11 +8001,11 @@
       <c r="L57" s="407"/>
       <c r="M57" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!S107,'Ranch Strategies'!S190)</f>
-        <v>501667.26264701999</v>
+        <v>512905.110721095</v>
       </c>
       <c r="N57" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!S190,'Ranch Strategies'!S107)</f>
-        <v>473111.14724279998</v>
+        <v>484348.99531687499</v>
       </c>
       <c r="Q57" s="155" t="s">
         <v>115</v>
@@ -7974,15 +8095,15 @@
       </c>
       <c r="S59" s="148">
         <f>'Ranch Strategies'!Q84</f>
-        <v>55138.572309009673</v>
+        <v>62597.842528418929</v>
       </c>
       <c r="T59" s="148">
         <f>'Ranch Strategies'!R84</f>
-        <v>-33275.741692702402</v>
+        <v>-13475.741692702402</v>
       </c>
       <c r="U59" s="148">
         <f>'Ranch Strategies'!S84</f>
-        <v>-28116.821692702419</v>
+        <v>-17358.679192702402</v>
       </c>
       <c r="V59" s="148">
         <f>'Ranch Strategies'!T84</f>
@@ -8011,15 +8132,15 @@
       </c>
       <c r="S60" s="148">
         <f>'Ranch Strategies'!Q99</f>
-        <v>31140.179757549762</v>
+        <v>31204.142999681197</v>
       </c>
       <c r="T60" s="148">
         <f>'Ranch Strategies'!R99</f>
-        <v>28504.443289974348</v>
+        <v>29791.443289974348</v>
       </c>
       <c r="U60" s="148">
         <f>'Ranch Strategies'!S99</f>
-        <v>28839.773089974347</v>
+        <v>29539.052352474348</v>
       </c>
       <c r="V60" s="148">
         <f>'Ranch Strategies'!T99</f>
@@ -8054,15 +8175,15 @@
       </c>
       <c r="S61" s="148">
         <f>'Ranch Strategies'!Q114</f>
-        <v>31407.20679897075</v>
+        <v>31471.718525903463</v>
       </c>
       <c r="T61" s="148">
         <f>'Ranch Strategies'!R114</f>
-        <v>29775.456416274305</v>
+        <v>30754.381355052752</v>
       </c>
       <c r="U61" s="148">
         <f>'Ranch Strategies'!S114</f>
-        <v>30125.738572056303</v>
+        <v>30703.680384013693</v>
       </c>
       <c r="V61" s="148">
         <f>'Ranch Strategies'!T114</f>
@@ -8081,11 +8202,11 @@
       <c r="L62" s="407"/>
       <c r="M62" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!Q121,'Ranch Strategies'!Q204)</f>
-        <v>590732.56778175372</v>
+        <v>595937.76098104648</v>
       </c>
       <c r="N62" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!Q204,'Ranch Strategies'!Q121)</f>
-        <v>577939.67787380412</v>
+        <v>583144.87107309687</v>
       </c>
       <c r="Q62" s="149">
         <f>'Ranch Strategies'!E123</f>
@@ -8097,15 +8218,15 @@
       </c>
       <c r="S62" s="148">
         <f>'Ranch Strategies'!Q128</f>
-        <v>31676.523597271924</v>
+        <v>31741.588512263086</v>
       </c>
       <c r="T62" s="148">
         <f>'Ranch Strategies'!R128</f>
-        <v>30751.169868822304</v>
+        <v>31018.100175172331</v>
       </c>
       <c r="U62" s="148">
         <f>'Ranch Strategies'!S128</f>
-        <v>30821.535491343137</v>
+        <v>30966.96444330661</v>
       </c>
       <c r="V62" s="148">
         <f>'Ranch Strategies'!T128</f>
@@ -8124,11 +8245,11 @@
       <c r="L63" s="407"/>
       <c r="M63" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!R121,'Ranch Strategies'!R204)</f>
-        <v>516704.26950578415</v>
+        <v>538058.69401378615</v>
       </c>
       <c r="N63" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!R204,'Ranch Strategies'!R121)</f>
-        <v>491562.02349668997</v>
+        <v>513167.15520506998</v>
       </c>
       <c r="Q63" s="149">
         <f>'Ranch Strategies'!E137</f>
@@ -8140,15 +8261,15 @@
       </c>
       <c r="S63" s="148">
         <f>'Ranch Strategies'!Q142</f>
-        <v>31948.149787118531</v>
+        <v>32013.77263375574</v>
       </c>
       <c r="T63" s="148">
         <f>'Ranch Strategies'!R142</f>
-        <v>31014.861150447457</v>
+        <v>31284.080384174435</v>
       </c>
       <c r="U63" s="148">
         <f>'Ranch Strategies'!S128</f>
-        <v>30821.535491343137</v>
+        <v>30966.96444330661</v>
       </c>
       <c r="V63" s="148">
         <f>'Ranch Strategies'!T142</f>
@@ -8167,11 +8288,11 @@
       <c r="L64" s="407"/>
       <c r="M64" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!S121,'Ranch Strategies'!S204)</f>
-        <v>522333.51930745062</v>
+        <v>533967.83546452841</v>
       </c>
       <c r="N64" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!S204,'Ranch Strategies'!S121)</f>
-        <v>497191.27329835645</v>
+        <v>508930.21701805445</v>
       </c>
     </row>
     <row r="65" spans="10:14" x14ac:dyDescent="0.2">
@@ -8236,11 +8357,11 @@
       <c r="L69" s="407"/>
       <c r="M69" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!Q135,'Ranch Strategies'!Q218)</f>
-        <v>612462.66296948225</v>
+        <v>617712.49070045887</v>
       </c>
       <c r="N69" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!Q218,'Ranch Strategies'!Q135)</f>
-        <v>604247.26061157195</v>
+        <v>609497.0883425487</v>
       </c>
     </row>
     <row r="70" spans="10:14" x14ac:dyDescent="0.2">
@@ -8251,11 +8372,11 @@
       <c r="L70" s="407"/>
       <c r="M70" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!R135,'Ranch Strategies'!R218)</f>
-        <v>537799.57203579624</v>
+        <v>559337.11073395447</v>
       </c>
       <c r="N70" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!R218,'Ranch Strategies'!R135)</f>
-        <v>516464.87412440742</v>
+        <v>538919.31356095348</v>
       </c>
     </row>
     <row r="71" spans="10:14" x14ac:dyDescent="0.2">
@@ -8266,11 +8387,11 @@
       <c r="L71" s="407"/>
       <c r="M71" s="416">
         <f>IF($G$51=1, 'Ranch Strategies'!S135,'Ranch Strategies'!S218)</f>
-        <v>543477.09265451203</v>
+        <v>555211.17307263671</v>
       </c>
       <c r="N71" s="417">
         <f>IF($G$51=1, 'Ranch Strategies'!S218,'Ranch Strategies'!S135)</f>
-        <v>522345.13217473013</v>
+        <v>534607.51539488952</v>
       </c>
     </row>
     <row r="72" spans="10:14" x14ac:dyDescent="0.2">
@@ -8335,11 +8456,11 @@
       <c r="L76" s="407"/>
       <c r="M76" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!Q149,'Ranch Strategies'!Q232)</f>
-        <v>634379.09372344555</v>
+        <v>639673.9387272154</v>
       </c>
       <c r="N76" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!Q232,'Ranch Strategies'!Q149)</f>
-        <v>630780.43087131623</v>
+        <v>636075.27587508596</v>
       </c>
     </row>
     <row r="77" spans="10:14" x14ac:dyDescent="0.2">
@@ -8350,11 +8471,11 @@
       <c r="L77" s="407"/>
       <c r="M77" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!R149,'Ranch Strategies'!R232)</f>
-        <v>559075.76678500324</v>
+        <v>580797.98987749801</v>
       </c>
       <c r="N77" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!R232,'Ranch Strategies'!R149)</f>
-        <v>542245.31042002421</v>
+        <v>564892.29667473864</v>
       </c>
     </row>
     <row r="78" spans="10:14" x14ac:dyDescent="0.2">
@@ -8365,11 +8486,11 @@
       <c r="L78" s="407"/>
       <c r="M78" s="416">
         <f>IF($G$51=1,'Ranch Strategies'!S149,'Ranch Strategies'!S232)</f>
-        <v>564801.97214302444</v>
+        <v>576636.67230073456</v>
       </c>
       <c r="N78" s="417">
         <f>IF($G$51=1,'Ranch Strategies'!S232,'Ranch Strategies'!S149)</f>
-        <v>548175.99168312841</v>
+        <v>560543.52483940066</v>
       </c>
     </row>
     <row r="79" spans="10:14" x14ac:dyDescent="0.2">
@@ -8430,8 +8551,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8478,19 +8599,19 @@
       <c r="C3"/>
       <c r="D3">
         <f>SUM(D16:O16)</f>
-        <v>0.52506122115640519</v>
+        <v>0.52236121052680584</v>
       </c>
       <c r="E3" s="172">
         <f>SUM(D17:O17)</f>
-        <v>0.86285919084859752</v>
+        <v>0.91934720965481176</v>
       </c>
       <c r="F3" s="172">
         <f>SUM(D18:O18)</f>
-        <v>0.77091180097417411</v>
+        <v>0.82714981978038837</v>
       </c>
       <c r="G3" s="172">
         <f>SUM(D19:O19)</f>
-        <v>0.74817432356158775</v>
+        <v>0.76114290573656729</v>
       </c>
       <c r="P3"/>
     </row>
@@ -8609,9 +8730,9 @@
         <f>IF($H$7&lt;$C$9,('CPER Precip'!F81),"#N/A")</f>
         <v>2.2273684210526317</v>
       </c>
-      <c r="I8" s="173" t="str">
+      <c r="I8" s="173">
         <f>IF($I$7&lt;$C$9,('CPER Precip'!G81),"#N/A")</f>
-        <v>#N/A</v>
+        <v>2.2528947368421059</v>
       </c>
       <c r="J8" s="173" t="str">
         <f>IF($J$7&lt;$C$9,('CPER Precip'!H81),"#N/A")</f>
@@ -8653,7 +8774,7 @@
       </c>
       <c r="C9" s="226">
         <f>UI!F9</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="172">
         <f>VLOOKUP($B$9, 'CPER Precip'!$A$2:$M$81,D7+1)</f>
@@ -8675,9 +8796,9 @@
         <f>IF($H$7&lt;$C$9,(VLOOKUP($B$9, 'CPER Precip'!$A$2:$M$81,H7+1)),"#N/A")</f>
         <v>1.27</v>
       </c>
-      <c r="I9" s="172" t="str">
+      <c r="I9" s="172">
         <f>IF($I$7&lt;$C$9,(VLOOKUP($B$9, 'CPER Precip'!$A$2:$M$81,I7+1)),"#N/A")</f>
-        <v>#N/A</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="J9" s="172" t="str">
         <f>IF($J$7&lt;$C$9,(VLOOKUP($B$9, 'CPER Precip'!$A$2:$M$81,J7+1)),"#N/A")</f>
@@ -8733,9 +8854,9 @@
         <f>IF($H$7&lt;$C$9,(H9/H8),"#N/A")</f>
         <v>0.57017958412098302</v>
       </c>
-      <c r="I10" s="172" t="str">
+      <c r="I10" s="172">
         <f>IF($I$7&lt;$C$9,(I9/I8), "#N/A")</f>
-        <v>#N/A</v>
+        <v>0.49713818479149624</v>
       </c>
       <c r="J10" s="172" t="str">
         <f>IF($J$7&lt;$C$9,(J9/J8),"#N/A")</f>
@@ -8988,7 +9109,7 @@
       </c>
       <c r="I16" s="172">
         <f>IF($I$7&lt;$C$9,(I11*I$10),IF($Q$9&gt;$I$7,0.049431,0.086547))</f>
-        <v>4.9431000000000003E-2</v>
+        <v>4.6730989370400648E-2</v>
       </c>
       <c r="J16" s="172">
         <f>IF($J$7&lt;$C$9,(J11*J$10), 0)</f>
@@ -9042,7 +9163,7 @@
       </c>
       <c r="I17" s="172">
         <f>IF($I$7&lt;$C$9,(I12*I$10), IF($Q$9&gt;$I$7,0.047911,0.118421))</f>
-        <v>4.7911000000000002E-2</v>
+        <v>0.1043990188062142</v>
       </c>
       <c r="J17" s="172">
         <f>IF($J$7&lt;$C$9,(J12*J$10), IF($Q$9&gt;$J$7,0.047911,0.118421))</f>
@@ -9096,7 +9217,7 @@
       </c>
       <c r="I18" s="172">
         <f>IF($I$7&lt;$C$9,(I13*I$10), IF($Q$9&gt;$I$7, 0.048161,0.099464))</f>
-        <v>4.8161000000000002E-2</v>
+        <v>0.1043990188062142</v>
       </c>
       <c r="J18" s="172">
         <f>IF($J$7&lt;$C$9,(J13*J$10),IF($Q$9&gt;$J$7,0.048161,0.099464))</f>
@@ -9150,7 +9271,7 @@
       </c>
       <c r="I19" s="172">
         <f>IF($I$7&lt;$C$9,(I14*I$10),IF($Q$9&gt;$I$7, 0.046688,0.109621))</f>
-        <v>4.6688E-2</v>
+        <v>5.9656582174979544E-2</v>
       </c>
       <c r="J19" s="172">
         <f>IF($J$7&lt;$C$9,(J14*J$10),IF($Q$9&gt;$J$7, 0.046688,0.109621))</f>
@@ -13546,7 +13667,7 @@
       </c>
       <c r="V11" s="470">
         <f>(($U$11-$U$10)*$I$13)+$U$10</f>
-        <v>548.45515521918924</v>
+        <v>561.10870945058741</v>
       </c>
       <c r="AH11" s="363"/>
       <c r="AI11" s="357"/>
@@ -13603,7 +13724,7 @@
       <c r="H13" s="67"/>
       <c r="I13" s="186">
         <f>'Drought Calculator'!F3</f>
-        <v>0.77091180097417411</v>
+        <v>0.82714981978038837</v>
       </c>
       <c r="J13" s="67"/>
       <c r="K13" s="67"/>
@@ -13760,11 +13881,11 @@
       <c r="Z16" s="273"/>
       <c r="AA16" s="273">
         <f>IF($U$19&lt;2, $U$18-I21, 12-I21)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AB16" s="274">
         <f>AA16*30</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="AH16" s="363"/>
       <c r="AJ16" s="357"/>
@@ -13953,7 +14074,7 @@
       </c>
       <c r="I21" s="157">
         <f>UI!F10</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J21" s="67"/>
       <c r="K21" s="67"/>
@@ -13971,11 +14092,11 @@
       <c r="Z21" s="134"/>
       <c r="AA21" s="134">
         <f>SUM(AA16:AA20)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AB21" s="276">
         <f>SUM(AB16:AB20)</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="AH21" s="363"/>
       <c r="AI21" s="357"/>
@@ -14144,18 +14265,18 @@
       <c r="N27" s="13"/>
       <c r="P27" s="326">
         <f>AB16</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
       <c r="S27" s="7"/>
       <c r="T27" s="253">
         <f>I29*P27</f>
-        <v>198.00000000000003</v>
+        <v>165</v>
       </c>
       <c r="U27" s="254">
         <f>T27*I8</f>
-        <v>118800.00000000001</v>
+        <v>99000</v>
       </c>
       <c r="W27" s="13"/>
     </row>
@@ -14209,18 +14330,18 @@
       <c r="N29" s="13"/>
       <c r="P29" s="328">
         <f>AB21</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
       <c r="T29" s="255">
         <f>I29*P29</f>
-        <v>198.00000000000003</v>
+        <v>165</v>
       </c>
       <c r="U29" s="256">
         <f>T29*I8</f>
-        <v>118800.00000000001</v>
+        <v>99000</v>
       </c>
       <c r="W29" s="13"/>
     </row>
@@ -14721,7 +14842,7 @@
       <c r="H46" s="79"/>
       <c r="I46" s="9">
         <f>AB16</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="N46" s="13"/>
       <c r="P46" s="135" t="s">
@@ -14766,11 +14887,11 @@
       <c r="S47" s="21"/>
       <c r="T47" s="63">
         <f>U47/$I$8</f>
-        <v>98.94</v>
+        <v>82.449999999999989</v>
       </c>
       <c r="U47" s="238">
         <f>(I45/30)*I46*I8</f>
-        <v>59364</v>
+        <v>49469.999999999993</v>
       </c>
       <c r="Y47" s="54" t="s">
         <v>75</v>
@@ -14874,7 +14995,7 @@
       <c r="H50" s="145"/>
       <c r="I50" s="297">
         <f>AB21</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="N50" s="13"/>
       <c r="P50" s="331" t="s">
@@ -14885,11 +15006,11 @@
       <c r="S50" s="22"/>
       <c r="T50" s="64">
         <f t="shared" si="3"/>
-        <v>5.9618000000000002</v>
+        <v>4.5215625000000008</v>
       </c>
       <c r="U50" s="242">
         <f>(U45+U46+U47+U48)*((I15/360)*I46)</f>
-        <v>3577.08</v>
+        <v>2712.9375000000005</v>
       </c>
       <c r="W50" s="13"/>
       <c r="Y50" s="54"/>
@@ -14910,7 +15031,7 @@
       <c r="H51" s="146"/>
       <c r="I51" s="298">
         <f>AA21</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N51" s="13"/>
       <c r="P51" s="332" t="s">
@@ -14921,11 +15042,11 @@
       <c r="S51" s="110"/>
       <c r="T51" s="111">
         <f>SUM(T45:T48, T50)</f>
-        <v>189.40180000000001</v>
+        <v>171.47156249999998</v>
       </c>
       <c r="U51" s="243">
         <f>SUM(U45:U48, U50)</f>
-        <v>113641.08</v>
+        <v>102882.9375</v>
       </c>
       <c r="W51" s="29"/>
       <c r="Y51" s="122" t="s">
@@ -14964,7 +15085,7 @@
       <c r="AB52" s="114"/>
       <c r="AC52" s="124">
         <f>AC51*AB16*(I16/360)</f>
-        <v>3187.5</v>
+        <v>2656.25</v>
       </c>
     </row>
     <row r="53" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14995,7 +15116,7 @@
       <c r="AB53" s="114"/>
       <c r="AC53" s="124">
         <f>(AC51+AC52)*I16</f>
-        <v>6414.84375</v>
+        <v>6408.203125</v>
       </c>
     </row>
     <row r="54" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15029,7 +15150,7 @@
       <c r="AB54" s="116"/>
       <c r="AC54" s="128">
         <f>(AC51+AC52+AC53)*I16</f>
-        <v>6495.029296875</v>
+        <v>6488.3056640625</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -15205,15 +15326,15 @@
       </c>
       <c r="Z58" s="148">
         <f t="shared" ref="Z58:AD58" si="5">Q92</f>
-        <v>547825.06060398067</v>
+        <v>552942.11997449538</v>
       </c>
       <c r="AA58" s="148">
         <f t="shared" si="5"/>
-        <v>476724.2583072976</v>
+        <v>496524.2583072976</v>
       </c>
       <c r="AB58" s="148">
         <f t="shared" si="5"/>
-        <v>481883.17830729758</v>
+        <v>492641.3208072976</v>
       </c>
       <c r="AC58" s="148">
         <f t="shared" si="5"/>
@@ -15244,11 +15365,11 @@
       <c r="S59" s="139"/>
       <c r="T59" s="25">
         <f>U59/I8</f>
-        <v>-5.3125</v>
+        <v>-4.427083333333333</v>
       </c>
       <c r="U59" s="247">
         <f>-(AC49*AB16*(I16/360))</f>
-        <v>-3187.5</v>
+        <v>-2656.25</v>
       </c>
       <c r="W59" s="13"/>
       <c r="X59" s="149">
@@ -15261,15 +15382,15 @@
       </c>
       <c r="Z59" s="148">
         <f t="shared" ref="Z59:AD59" si="6">Q107</f>
-        <v>569187.22391765972</v>
+        <v>574348.1620722767</v>
       </c>
       <c r="AA59" s="148">
         <f t="shared" si="6"/>
-        <v>496278.30640422</v>
+        <v>516961.18840421998</v>
       </c>
       <c r="AB59" s="148">
         <f t="shared" si="6"/>
-        <v>501667.26264701999</v>
+        <v>512905.110721095</v>
       </c>
       <c r="AC59" s="148">
         <f t="shared" si="6"/>
@@ -15298,11 +15419,11 @@
       <c r="S60" s="140"/>
       <c r="T60" s="141">
         <f>SUM(T56:T59)</f>
-        <v>193.0625</v>
+        <v>193.94791666666666</v>
       </c>
       <c r="U60" s="248">
         <f>SUM(U56:U59)</f>
-        <v>115837.5</v>
+        <v>116368.75</v>
       </c>
       <c r="W60" s="13"/>
       <c r="X60" s="149">
@@ -15315,15 +15436,15 @@
       </c>
       <c r="Z60" s="148">
         <f>Q121</f>
-        <v>590732.56778175372</v>
+        <v>595937.76098104648</v>
       </c>
       <c r="AA60" s="148">
         <f>R121</f>
-        <v>516704.26950578415</v>
+        <v>538058.69401378615</v>
       </c>
       <c r="AB60" s="148">
         <f>S121</f>
-        <v>522333.51930745062</v>
+        <v>533967.83546452841</v>
       </c>
       <c r="AC60" s="148">
         <f>T121</f>
@@ -15369,15 +15490,15 @@
       </c>
       <c r="Z61" s="148">
         <f>Q135</f>
-        <v>612462.66296948225</v>
+        <v>617712.49070045887</v>
       </c>
       <c r="AA61" s="148">
         <f>R135</f>
-        <v>537799.57203579624</v>
+        <v>559337.11073395447</v>
       </c>
       <c r="AB61" s="148">
         <f>S135</f>
-        <v>543477.09265451203</v>
+        <v>555211.17307263671</v>
       </c>
       <c r="AC61" s="148">
         <f>T135</f>
@@ -15406,11 +15527,11 @@
       <c r="S62" s="23"/>
       <c r="T62" s="24">
         <f>U62/I8</f>
-        <v>-26.828955078124999</v>
+        <v>-25.9212646484375</v>
       </c>
       <c r="U62" s="246">
         <f>-(AC52+AC53+AC54)</f>
-        <v>-16097.373046875</v>
+        <v>-15552.7587890625</v>
       </c>
       <c r="W62" s="13"/>
       <c r="X62" s="149">
@@ -15423,15 +15544,15 @@
       </c>
       <c r="Z62" s="148">
         <f>Q149</f>
-        <v>634379.09372344555</v>
+        <v>639673.9387272154</v>
       </c>
       <c r="AA62" s="148">
         <f>R149</f>
-        <v>559075.76678500324</v>
+        <v>580797.98987749801</v>
       </c>
       <c r="AB62" s="148">
         <f>S149</f>
-        <v>564801.97214302444</v>
+        <v>576636.67230073456</v>
       </c>
       <c r="AC62" s="148">
         <f>T149</f>
@@ -15541,11 +15662,11 @@
       <c r="S66" s="23"/>
       <c r="T66" s="24">
         <f>SUM(T61:T65)</f>
-        <v>136.08771158854165</v>
+        <v>136.99540201822913</v>
       </c>
       <c r="U66" s="246">
         <f>SUM(U61:U65)</f>
-        <v>81652.626953125</v>
+        <v>82197.2412109375</v>
       </c>
       <c r="W66" s="13"/>
     </row>
@@ -15568,11 +15689,11 @@
       <c r="S67" s="142"/>
       <c r="T67" s="143">
         <f>T60+T66</f>
-        <v>329.15021158854165</v>
+        <v>330.94331868489576</v>
       </c>
       <c r="U67" s="249">
         <f>U60+U66</f>
-        <v>197490.126953125</v>
+        <v>198565.9912109375</v>
       </c>
       <c r="W67" s="13"/>
     </row>
@@ -15976,7 +16097,7 @@
       </c>
       <c r="Q81" s="89">
         <f>IF($I$22=E80,($I$8*$U$9)*$V$11*$U$14,($I$8*$U$9)*$U$11*$U$14)</f>
-        <v>323314.31400171207</v>
+        <v>330773.58422112133</v>
       </c>
       <c r="R81" s="90">
         <f>($I$8*$U$9)*$U$11*$U$14</f>
@@ -16065,11 +16186,11 @@
       </c>
       <c r="R83" s="94">
         <f>-IF(I19=1,(I8*I12)+(AB16*I29*I8)+U33, (I8*I12)+(AB16*I29*I8))</f>
-        <v>-425632.6335</v>
+        <v>-405832.6335</v>
       </c>
       <c r="S83" s="94">
         <f>-IF(I19=1, ((I8*I12)+U51)+(U33), ((I8*I12)+U51))</f>
-        <v>-420473.71350000001</v>
+        <v>-409715.571</v>
       </c>
       <c r="T83" s="94">
         <f>-IF(I19 = 1, (I8*(I12-I54))+(U33), (I8*(I12-I54)))</f>
@@ -16103,15 +16224,15 @@
       </c>
       <c r="Q84" s="90">
         <f t="shared" si="15"/>
-        <v>55138.572309009673</v>
+        <v>62597.842528418929</v>
       </c>
       <c r="R84" s="90">
         <f t="shared" si="15"/>
-        <v>-33275.741692702402</v>
+        <v>-13475.741692702402</v>
       </c>
       <c r="S84" s="90">
         <f t="shared" si="15"/>
-        <v>-28116.821692702419</v>
+        <v>-17358.679192702402</v>
       </c>
       <c r="T84" s="90">
         <f t="shared" si="15"/>
@@ -16166,7 +16287,7 @@
       </c>
       <c r="Q85" s="95">
         <f t="shared" si="16"/>
-        <v>17313.511705029036</v>
+        <v>19655.722553923544</v>
       </c>
       <c r="R85" s="95">
         <f t="shared" si="16"/>
@@ -16235,15 +16356,15 @@
       </c>
       <c r="Q86" s="97">
         <f t="shared" si="18"/>
-        <v>37825.060603980637</v>
+        <v>42942.119974495385</v>
       </c>
       <c r="R86" s="97">
         <f t="shared" si="18"/>
-        <v>-33275.741692702402</v>
+        <v>-13475.741692702402</v>
       </c>
       <c r="S86" s="97">
         <f t="shared" si="18"/>
-        <v>-28116.821692702419</v>
+        <v>-17358.679192702402</v>
       </c>
       <c r="T86" s="97">
         <f t="shared" si="18"/>
@@ -16264,15 +16385,15 @@
       </c>
       <c r="Z86" s="148">
         <f t="shared" si="19"/>
-        <v>55138.572309009673</v>
+        <v>62597.842528418929</v>
       </c>
       <c r="AA86" s="148">
         <f t="shared" si="19"/>
-        <v>-33275.741692702402</v>
+        <v>-13475.741692702402</v>
       </c>
       <c r="AB86" s="148">
         <f t="shared" si="19"/>
-        <v>-28116.821692702419</v>
+        <v>-17358.679192702402</v>
       </c>
       <c r="AC86" s="148">
         <f t="shared" si="19"/>
@@ -16330,15 +16451,15 @@
       </c>
       <c r="Z87" s="148">
         <f t="shared" si="20"/>
-        <v>31140.179757549762</v>
+        <v>31204.142999681197</v>
       </c>
       <c r="AA87" s="148">
         <f t="shared" si="20"/>
-        <v>28504.443289974348</v>
+        <v>29791.443289974348</v>
       </c>
       <c r="AB87" s="148">
         <f t="shared" si="20"/>
-        <v>28839.773089974347</v>
+        <v>29539.052352474348</v>
       </c>
       <c r="AC87" s="148">
         <f t="shared" si="20"/>
@@ -16395,15 +16516,15 @@
       </c>
       <c r="Z88" s="148">
         <f>Q114</f>
-        <v>31407.20679897075</v>
+        <v>31471.718525903463</v>
       </c>
       <c r="AA88" s="148">
         <f>R114</f>
-        <v>29775.456416274305</v>
+        <v>30754.381355052752</v>
       </c>
       <c r="AB88" s="148">
         <f>S114</f>
-        <v>30125.738572056303</v>
+        <v>30703.680384013693</v>
       </c>
       <c r="AC88" s="148">
         <f>T114</f>
@@ -16447,15 +16568,15 @@
       </c>
       <c r="Z89" s="148">
         <f>Q128</f>
-        <v>31676.523597271924</v>
+        <v>31741.588512263086</v>
       </c>
       <c r="AA89" s="148">
         <f>R128</f>
-        <v>30751.169868822304</v>
+        <v>31018.100175172331</v>
       </c>
       <c r="AB89" s="148">
         <f>S128</f>
-        <v>30821.535491343137</v>
+        <v>30966.96444330661</v>
       </c>
       <c r="AC89" s="148">
         <f>T128</f>
@@ -16517,15 +16638,15 @@
       </c>
       <c r="Z90" s="148">
         <f>Q142</f>
-        <v>31948.149787118531</v>
+        <v>32013.77263375574</v>
       </c>
       <c r="AA90" s="148">
         <f>R142</f>
-        <v>31014.861150447457</v>
+        <v>31284.080384174435</v>
       </c>
       <c r="AB90" s="148">
         <f>S142</f>
-        <v>31085.830158181405</v>
+        <v>31232.506163407961</v>
       </c>
       <c r="AC90" s="148">
         <f>T142</f>
@@ -16558,15 +16679,15 @@
       </c>
       <c r="Q91" s="87">
         <f t="shared" ref="Q91:U91" si="25">Q86+Q87-Q88</f>
-        <v>37825.060603980637</v>
+        <v>42942.119974495385</v>
       </c>
       <c r="R91" s="87">
         <f t="shared" si="25"/>
-        <v>-33275.741692702402</v>
+        <v>-13475.741692702402</v>
       </c>
       <c r="S91" s="87">
         <f t="shared" si="25"/>
-        <v>-28116.821692702419</v>
+        <v>-17358.679192702402</v>
       </c>
       <c r="T91" s="87">
         <f t="shared" si="25"/>
@@ -16600,15 +16721,15 @@
       </c>
       <c r="Q92" s="265">
         <f>SUM(Q90:Q91)</f>
-        <v>547825.06060398067</v>
+        <v>552942.11997449538</v>
       </c>
       <c r="R92" s="265">
         <f>SUM(R90:R91)</f>
-        <v>476724.2583072976</v>
+        <v>496524.2583072976</v>
       </c>
       <c r="S92" s="265">
         <f t="shared" ref="S92" si="26">SUM(S90:S91)</f>
-        <v>481883.17830729758</v>
+        <v>492641.3208072976</v>
       </c>
       <c r="T92" s="265">
         <f>SUM(T90:T91)</f>
@@ -16813,15 +16934,15 @@
       </c>
       <c r="Q98" s="94">
         <f t="shared" si="28"/>
-        <v>472.81325754975796</v>
+        <v>536.77649968119238</v>
       </c>
       <c r="R98" s="94">
         <f t="shared" si="28"/>
-        <v>-2162.9232100256563</v>
+        <v>-875.9232100256562</v>
       </c>
       <c r="S98" s="94">
         <f t="shared" si="28"/>
-        <v>-1827.5934100256572</v>
+        <v>-1128.3141475256562</v>
       </c>
       <c r="T98" s="94">
         <f t="shared" si="28"/>
@@ -16855,15 +16976,15 @@
       </c>
       <c r="Q99" s="90">
         <f t="shared" si="29"/>
-        <v>31140.179757549762</v>
+        <v>31204.142999681197</v>
       </c>
       <c r="R99" s="90">
         <f t="shared" si="29"/>
-        <v>28504.443289974348</v>
+        <v>29791.443289974348</v>
       </c>
       <c r="S99" s="90">
         <f t="shared" si="29"/>
-        <v>28839.773089974347</v>
+        <v>29539.052352474348</v>
       </c>
       <c r="T99" s="90">
         <f t="shared" si="29"/>
@@ -16897,15 +17018,15 @@
       </c>
       <c r="Q100" s="95">
         <f t="shared" si="30"/>
-        <v>9778.0164438706252</v>
+        <v>9798.1009018998957</v>
       </c>
       <c r="R100" s="95">
         <f t="shared" si="30"/>
-        <v>8950.3951930519452</v>
+        <v>9354.5131930519456</v>
       </c>
       <c r="S100" s="95">
         <f t="shared" si="30"/>
-        <v>9055.6887502519457</v>
+        <v>9275.2624386769457</v>
       </c>
       <c r="T100" s="95">
         <f t="shared" si="30"/>
@@ -16939,15 +17060,15 @@
       </c>
       <c r="Q101" s="97">
         <f>Q99-Q100</f>
-        <v>21362.163313679135</v>
+        <v>21406.042097781301</v>
       </c>
       <c r="R101" s="97">
         <f t="shared" ref="R101:S101" si="31">R99-R100</f>
-        <v>19554.048096922401</v>
+        <v>20436.930096922402</v>
       </c>
       <c r="S101" s="102">
         <f t="shared" si="31"/>
-        <v>19784.084339722402</v>
+        <v>20263.789913797402</v>
       </c>
       <c r="T101" s="97">
         <f>T99-T100</f>
@@ -17106,15 +17227,15 @@
       </c>
       <c r="Q106" s="103">
         <f>Q91+Q101</f>
-        <v>59187.223917659772</v>
+        <v>64348.162072276682</v>
       </c>
       <c r="R106" s="103">
         <f>R91+R101</f>
-        <v>-13721.693595780001</v>
+        <v>6961.1884042199999</v>
       </c>
       <c r="S106" s="103">
         <f>S91+S101</f>
-        <v>-8332.737352980017</v>
+        <v>2905.1107210949995</v>
       </c>
       <c r="T106" s="103">
         <f>T91+T101-T102</f>
@@ -17148,15 +17269,15 @@
       </c>
       <c r="Q107" s="310">
         <f>SUM(Q105:Q106)</f>
-        <v>569187.22391765972</v>
+        <v>574348.1620722767</v>
       </c>
       <c r="R107" s="310">
         <f t="shared" ref="R107:S107" si="33">SUM(R105:R106)</f>
-        <v>496278.30640422</v>
+        <v>516961.18840421998</v>
       </c>
       <c r="S107" s="310">
         <f t="shared" si="33"/>
-        <v>501667.26264701999</v>
+        <v>512905.110721095</v>
       </c>
       <c r="T107" s="310">
         <f>SUM(T105:T106)</f>
@@ -17361,15 +17482,15 @@
       </c>
       <c r="Q113" s="94">
         <f t="shared" si="34"/>
-        <v>739.8402989707472</v>
+        <v>804.35202590345853</v>
       </c>
       <c r="R113" s="94">
         <f t="shared" si="34"/>
-        <v>-891.91008372570013</v>
+        <v>87.014855052750008</v>
       </c>
       <c r="S113" s="94">
         <f t="shared" si="34"/>
-        <v>-541.62792794370114</v>
+        <v>36.313884013687492</v>
       </c>
       <c r="T113" s="94">
         <f t="shared" si="34"/>
@@ -17403,15 +17524,15 @@
       </c>
       <c r="Q114" s="90">
         <f>SUM(Q110:Q113)</f>
-        <v>31407.20679897075</v>
+        <v>31471.718525903463</v>
       </c>
       <c r="R114" s="90">
         <f>SUM(R110:R113)</f>
-        <v>29775.456416274305</v>
+        <v>30754.381355052752</v>
       </c>
       <c r="S114" s="90">
         <f>SUM(S110:S113)</f>
-        <v>30125.738572056303</v>
+        <v>30703.680384013693</v>
       </c>
       <c r="T114" s="90">
         <f>SUM(T110:T113)</f>
@@ -17445,15 +17566,15 @@
       </c>
       <c r="Q115" s="95">
         <f>IF(Q114&gt;0,Q114*(0.124+0.15+0.04),0)</f>
-        <v>9861.8629348768154</v>
+        <v>9882.1196171336869</v>
       </c>
       <c r="R115" s="95">
         <f>IF(R114&gt;0,R114*(0.124+0.15+0.04),0)</f>
-        <v>9349.493314710131</v>
+        <v>9656.8757454865645</v>
       </c>
       <c r="S115" s="95">
         <f>IF(S114&gt;0,S114*(0.124+0.15+0.04),0)</f>
-        <v>9459.4819116256785</v>
+        <v>9640.9556405802996</v>
       </c>
       <c r="T115" s="95">
         <f>IF(T114&gt;0,T114*(0.124+0.15+0.04),0)</f>
@@ -17487,15 +17608,15 @@
       </c>
       <c r="Q116" s="97">
         <f t="shared" si="37"/>
-        <v>21545.343864093935</v>
+        <v>21589.598908769774</v>
       </c>
       <c r="R116" s="97">
         <f t="shared" si="37"/>
-        <v>20425.963101564172</v>
+        <v>21097.505609566186</v>
       </c>
       <c r="S116" s="97">
         <f t="shared" si="37"/>
-        <v>20666.256660430627</v>
+        <v>21062.724743433391</v>
       </c>
       <c r="T116" s="97">
         <f t="shared" si="37"/>
@@ -17632,15 +17753,15 @@
       </c>
       <c r="Q120" s="103">
         <f>Q106+Q116-Q117</f>
-        <v>80732.567781753707</v>
+        <v>85937.760981046449</v>
       </c>
       <c r="R120" s="103">
         <f>R106+R116-R117</f>
-        <v>6704.2695057841702</v>
+        <v>28058.694013786186</v>
       </c>
       <c r="S120" s="103">
         <f>S106+S116-S117</f>
-        <v>12333.51930745061</v>
+        <v>23967.835464528391</v>
       </c>
       <c r="T120" s="103">
         <f>T106+T116-T117</f>
@@ -17674,15 +17795,15 @@
       </c>
       <c r="Q121" s="310">
         <f t="shared" si="40"/>
-        <v>590732.56778175372</v>
+        <v>595937.76098104648</v>
       </c>
       <c r="R121" s="310">
         <f t="shared" si="40"/>
-        <v>516704.26950578415</v>
+        <v>538058.69401378615</v>
       </c>
       <c r="S121" s="310">
         <f t="shared" si="40"/>
-        <v>522333.51930745062</v>
+        <v>533967.83546452841</v>
       </c>
       <c r="T121" s="310">
         <f t="shared" si="40"/>
@@ -17887,15 +18008,15 @@
       </c>
       <c r="Q127" s="94">
         <f>IF(Q120&gt;0,Q120*$I$16,Q120*$I$15)</f>
-        <v>1009.1570972719214</v>
+        <v>1074.2220122630806</v>
       </c>
       <c r="R127" s="94">
         <f>IF(R120&gt;0,R120*$I$16,R120*$I$15)</f>
-        <v>83.803368822302133</v>
+        <v>350.73367517232737</v>
       </c>
       <c r="S127" s="94">
         <f>IF(S120&gt;0,S120*$I$16,S120*$I$15)</f>
-        <v>154.16899134313263</v>
+        <v>299.59794330660492</v>
       </c>
       <c r="T127" s="94">
         <f>IF(T120&gt;0,T120*$I$16,T120*$I$15)</f>
@@ -17929,15 +18050,15 @@
       </c>
       <c r="Q128" s="90">
         <f>SUM(Q124:Q127)</f>
-        <v>31676.523597271924</v>
+        <v>31741.588512263086</v>
       </c>
       <c r="R128" s="90">
         <f>SUM(R124:R127)</f>
-        <v>30751.169868822304</v>
+        <v>31018.100175172331</v>
       </c>
       <c r="S128" s="90">
         <f>SUM(S124:S127)</f>
-        <v>30821.535491343137</v>
+        <v>30966.96444330661</v>
       </c>
       <c r="T128" s="90">
         <f>SUM(T124:T127)</f>
@@ -17971,15 +18092,15 @@
       </c>
       <c r="Q129" s="95">
         <f>IF(Q128&gt;0,Q128*(0.124+0.15+0.04),0)</f>
-        <v>9946.428409543385</v>
+        <v>9966.8587928506095</v>
       </c>
       <c r="R129" s="95">
         <f>IF(R128&gt;0,R128*(0.124+0.15+0.04),0)</f>
-        <v>9655.8673388102034</v>
+        <v>9739.6834550041112</v>
       </c>
       <c r="S129" s="95">
         <f>IF(S128&gt;0,S128*(0.124+0.15+0.04),0)</f>
-        <v>9677.9621442817443</v>
+        <v>9723.6268351982762</v>
       </c>
       <c r="T129" s="95">
         <f>IF(T128&gt;0,T128*(0.124+0.15+0.04),0)</f>
@@ -18013,15 +18134,15 @@
       </c>
       <c r="Q130" s="97">
         <f t="shared" si="44"/>
-        <v>21730.095187728541</v>
+        <v>21774.729719412477</v>
       </c>
       <c r="R130" s="97">
         <f t="shared" si="44"/>
-        <v>21095.302530012101</v>
+        <v>21278.416720168221</v>
       </c>
       <c r="S130" s="97">
         <f t="shared" si="44"/>
-        <v>21143.573347061392</v>
+        <v>21243.337608108333</v>
       </c>
       <c r="T130" s="97">
         <f t="shared" si="44"/>
@@ -18158,15 +18279,15 @@
       </c>
       <c r="Q134" s="103">
         <f>Q120+Q130-Q131</f>
-        <v>102462.66296948225</v>
+        <v>107712.49070045893</v>
       </c>
       <c r="R134" s="103">
         <f>R120+R130-R131</f>
-        <v>27799.572035796271</v>
+        <v>49337.110733954411</v>
       </c>
       <c r="S134" s="103">
         <f>S120+S130-S131</f>
-        <v>33477.092654512002</v>
+        <v>45211.173072636724</v>
       </c>
       <c r="T134" s="103">
         <f>T120+T130-T131</f>
@@ -18200,15 +18321,15 @@
       </c>
       <c r="Q135" s="310">
         <f t="shared" si="47"/>
-        <v>612462.66296948225</v>
+        <v>617712.49070045887</v>
       </c>
       <c r="R135" s="310">
         <f t="shared" si="47"/>
-        <v>537799.57203579624</v>
+        <v>559337.11073395447</v>
       </c>
       <c r="S135" s="310">
         <f t="shared" si="47"/>
-        <v>543477.09265451203</v>
+        <v>555211.17307263671</v>
       </c>
       <c r="T135" s="310">
         <f t="shared" si="47"/>
@@ -18411,15 +18532,15 @@
       </c>
       <c r="Q141" s="94">
         <f>IF(Q134&gt;0,Q134*$I$16,Q134*$I$15)</f>
-        <v>1280.7832871185283</v>
+        <v>1346.4061337557368</v>
       </c>
       <c r="R141" s="94">
         <f>IF(R134&gt;0,R134*$I$16,R134*$I$15)</f>
-        <v>347.49465044745341</v>
+        <v>616.71388417443018</v>
       </c>
       <c r="S141" s="94">
         <f>IF(S134&gt;0,S134*$I$16,S134*$I$15)</f>
-        <v>418.46365818140004</v>
+        <v>565.13966340795912</v>
       </c>
       <c r="T141" s="94">
         <f>IF(T134&gt;0,T134*$I$16,T134*$I$15)</f>
@@ -18452,15 +18573,15 @@
       </c>
       <c r="Q142" s="90">
         <f>SUM(Q138:Q141)</f>
-        <v>31948.149787118531</v>
+        <v>32013.77263375574</v>
       </c>
       <c r="R142" s="90">
         <f>SUM(R138:R141)</f>
-        <v>31014.861150447457</v>
+        <v>31284.080384174435</v>
       </c>
       <c r="S142" s="90">
         <f>SUM(S138:S141)</f>
-        <v>31085.830158181405</v>
+        <v>31232.506163407961</v>
       </c>
       <c r="T142" s="90">
         <f>SUM(T138:T141)</f>
@@ -18493,15 +18614,15 @@
       </c>
       <c r="Q143" s="95">
         <f>IF(Q142&gt;0,Q142*(0.124+0.15+0.04),0)</f>
-        <v>10031.719033155219</v>
+        <v>10052.324606999302</v>
       </c>
       <c r="R143" s="95">
         <f>IF(R142&gt;0,R142*(0.124+0.15+0.04),0)</f>
-        <v>9738.6664012405017</v>
+        <v>9823.2012406307731</v>
       </c>
       <c r="S143" s="95">
         <f>IF(S142&gt;0,S142*(0.124+0.15+0.04),0)</f>
-        <v>9760.9506696689605</v>
+        <v>9807.0069353101007</v>
       </c>
       <c r="T143" s="95">
         <f>IF(T142&gt;0,T142*(0.124+0.15+0.04),0)</f>
@@ -18534,15 +18655,15 @@
       </c>
       <c r="Q144" s="97">
         <f t="shared" si="51"/>
-        <v>21916.430753963312</v>
+        <v>21961.448026756436</v>
       </c>
       <c r="R144" s="97">
         <f t="shared" si="51"/>
-        <v>21276.194749206956</v>
+        <v>21460.879143543661</v>
       </c>
       <c r="S144" s="97">
         <f t="shared" si="51"/>
-        <v>21324.879488512444</v>
+        <v>21425.499228097862</v>
       </c>
       <c r="T144" s="97">
         <f t="shared" si="51"/>
@@ -18675,15 +18796,15 @@
       </c>
       <c r="Q148" s="103">
         <f>Q134+Q144-Q145</f>
-        <v>124379.09372344556</v>
+        <v>129673.93872721537</v>
       </c>
       <c r="R148" s="103">
         <f>R134+R144-R145</f>
-        <v>49075.76678500323</v>
+        <v>70797.989877498068</v>
       </c>
       <c r="S148" s="103">
         <f>S134+S144-S145</f>
-        <v>54801.972143024446</v>
+        <v>66636.672300734586</v>
       </c>
       <c r="T148" s="103">
         <f>T134+T144-T145</f>
@@ -18716,15 +18837,15 @@
       </c>
       <c r="Q149" s="310">
         <f t="shared" ref="Q149:U149" si="54">SUM(Q147:Q148)</f>
-        <v>634379.09372344555</v>
+        <v>639673.9387272154</v>
       </c>
       <c r="R149" s="310">
         <f t="shared" si="54"/>
-        <v>559075.76678500324</v>
+        <v>580797.98987749801</v>
       </c>
       <c r="S149" s="310">
         <f t="shared" si="54"/>
-        <v>564801.97214302444</v>
+        <v>576636.67230073456</v>
       </c>
       <c r="T149" s="310">
         <f t="shared" si="54"/>
@@ -18801,15 +18922,15 @@
       </c>
       <c r="Q152" s="322">
         <f t="shared" si="55"/>
-        <v>119691.59372344555</v>
+        <v>124986.4387272154</v>
       </c>
       <c r="R152" s="322">
         <f t="shared" si="55"/>
-        <v>44388.266785003245</v>
+        <v>66110.48987749801</v>
       </c>
       <c r="S152" s="322">
         <f t="shared" si="55"/>
-        <v>50114.472143024439</v>
+        <v>61949.172300734557</v>
       </c>
       <c r="T152" s="322">
         <f t="shared" si="55"/>
@@ -18842,15 +18963,15 @@
       </c>
       <c r="Q153" s="320">
         <f t="shared" si="56"/>
-        <v>199.48598953907592</v>
+        <v>208.31073121202567</v>
       </c>
       <c r="R153" s="320">
         <f t="shared" si="56"/>
-        <v>73.980444641672079</v>
+        <v>110.18414979583002</v>
       </c>
       <c r="S153" s="320">
         <f t="shared" si="56"/>
-        <v>83.524120238374067</v>
+        <v>103.24862050122427</v>
       </c>
       <c r="T153" s="320">
         <f t="shared" si="56"/>
@@ -19178,7 +19299,7 @@
       </c>
       <c r="Q164" s="89">
         <f>IF($I$22=E163,($I$8*$U$9)*$V$11*$U$14,($I$8*$U$9)*$U$11*$U$14)</f>
-        <v>323314.31400171207</v>
+        <v>330773.58422112133</v>
       </c>
       <c r="R164" s="90">
         <f>($I$8*$U$9)*$U$11*$U$14</f>
@@ -19265,11 +19386,11 @@
       </c>
       <c r="R166" s="94">
         <f>-IF(I19=1, (I8*I12)+(AB16*I29*I8),(I8*I12)+(AB16*I29*I8)+U33)</f>
-        <v>-418800</v>
+        <v>-399000</v>
       </c>
       <c r="S166" s="94">
         <f>-IF(I19=1, ((I8*I12)+U51), ((I8*I12)+U51)+(U33))</f>
-        <v>-413641.08</v>
+        <v>-402882.9375</v>
       </c>
       <c r="T166" s="94">
         <f>-IF(I19 = 1, (I8*(I12-I54)), (I8*(I12-I54))+(U33))</f>
@@ -19303,15 +19424,15 @@
       </c>
       <c r="Q167" s="90">
         <f t="shared" si="61"/>
-        <v>23314.314001712075</v>
+        <v>30773.584221121331</v>
       </c>
       <c r="R167" s="90">
         <f t="shared" si="61"/>
-        <v>-65100</v>
+        <v>-45300</v>
       </c>
       <c r="S167" s="90">
         <f t="shared" si="61"/>
-        <v>-59941.080000000016</v>
+        <v>-49182.9375</v>
       </c>
       <c r="T167" s="90">
         <f t="shared" si="61"/>
@@ -19345,7 +19466,7 @@
       </c>
       <c r="Q168" s="95">
         <f t="shared" si="62"/>
-        <v>7320.6945965375917</v>
+        <v>9662.9054454320976</v>
       </c>
       <c r="R168" s="95">
         <f t="shared" si="62"/>
@@ -19385,15 +19506,15 @@
       </c>
       <c r="Q169" s="97">
         <f t="shared" si="63"/>
-        <v>15993.619405174482</v>
+        <v>21110.678775689234</v>
       </c>
       <c r="R169" s="97">
         <f t="shared" si="63"/>
-        <v>-65100</v>
+        <v>-45300</v>
       </c>
       <c r="S169" s="97">
         <f t="shared" si="63"/>
-        <v>-59941.080000000016</v>
+        <v>-49182.9375</v>
       </c>
       <c r="T169" s="97">
         <f t="shared" si="63"/>
@@ -19558,15 +19679,15 @@
       </c>
       <c r="Q174" s="424">
         <f t="shared" ref="Q174:U174" si="65">Q169+Q170-Q171</f>
-        <v>15993.619405174482</v>
+        <v>21110.678775689234</v>
       </c>
       <c r="R174" s="424">
         <f t="shared" si="65"/>
-        <v>-65100</v>
+        <v>-45300</v>
       </c>
       <c r="S174" s="424">
         <f t="shared" si="65"/>
-        <v>-59941.080000000016</v>
+        <v>-49182.9375</v>
       </c>
       <c r="T174" s="424">
         <f t="shared" si="65"/>
@@ -19598,15 +19719,15 @@
       </c>
       <c r="Q175" s="265">
         <f>SUM(Q173:Q174)</f>
-        <v>525993.61940517451</v>
+        <v>531110.67877568922</v>
       </c>
       <c r="R175" s="265">
         <f>SUM(R173:R174)</f>
-        <v>444900</v>
+        <v>464700</v>
       </c>
       <c r="S175" s="265">
         <f t="shared" ref="S175" si="66">SUM(S173:S174)</f>
-        <v>450058.92</v>
+        <v>460817.0625</v>
       </c>
       <c r="T175" s="265">
         <f>SUM(T173:T174)</f>
@@ -19797,15 +19918,15 @@
       </c>
       <c r="Q181" s="94">
         <f t="shared" si="68"/>
-        <v>199.92024256468105</v>
+        <v>263.88348469611543</v>
       </c>
       <c r="R181" s="94">
         <f t="shared" si="68"/>
-        <v>-4231.5</v>
+        <v>-2944.5</v>
       </c>
       <c r="S181" s="94">
         <f t="shared" si="68"/>
-        <v>-3896.1702000000014</v>
+        <v>-3196.8909375000003</v>
       </c>
       <c r="T181" s="94">
         <f t="shared" si="68"/>
@@ -19836,15 +19957,15 @@
       </c>
       <c r="Q182" s="90">
         <f t="shared" si="69"/>
-        <v>37699.92024256468</v>
+        <v>37763.883484696118</v>
       </c>
       <c r="R182" s="90">
         <f t="shared" si="69"/>
-        <v>33268.5</v>
+        <v>34555.5</v>
       </c>
       <c r="S182" s="90">
         <f t="shared" si="69"/>
-        <v>33603.8298</v>
+        <v>34303.1090625</v>
       </c>
       <c r="T182" s="90">
         <f t="shared" si="69"/>
@@ -19875,15 +19996,15 @@
       </c>
       <c r="Q183" s="95">
         <f t="shared" si="70"/>
-        <v>11837.774956165309</v>
+        <v>11857.859414194581</v>
       </c>
       <c r="R183" s="95">
         <f t="shared" si="70"/>
-        <v>10446.308999999999</v>
+        <v>10850.427</v>
       </c>
       <c r="S183" s="95">
         <f t="shared" si="70"/>
-        <v>10551.6025572</v>
+        <v>10771.176245625</v>
       </c>
       <c r="T183" s="95">
         <f t="shared" si="70"/>
@@ -19914,15 +20035,15 @@
       </c>
       <c r="Q184" s="97">
         <f>Q182-Q183</f>
-        <v>25862.145286399369</v>
+        <v>25906.024070501539</v>
       </c>
       <c r="R184" s="97">
         <f t="shared" ref="R184:S184" si="71">R182-R183</f>
-        <v>22822.190999999999</v>
+        <v>23705.073</v>
       </c>
       <c r="S184" s="102">
         <f t="shared" si="71"/>
-        <v>23052.2272428</v>
+        <v>23531.932816875</v>
       </c>
       <c r="T184" s="97">
         <f>T182-T183</f>
@@ -20066,15 +20187,15 @@
       </c>
       <c r="Q189" s="430">
         <f>Q174+Q184</f>
-        <v>41855.764691573851</v>
+        <v>47016.702846190776</v>
       </c>
       <c r="R189" s="430">
         <f>R174+R184</f>
-        <v>-42277.809000000001</v>
+        <v>-21594.927</v>
       </c>
       <c r="S189" s="430">
         <f>S174+S184</f>
-        <v>-36888.852757200017</v>
+        <v>-25651.004683125</v>
       </c>
       <c r="T189" s="430">
         <f>T174+T184-T185</f>
@@ -20105,15 +20226,15 @@
       </c>
       <c r="Q190" s="310">
         <f>SUM(Q188:Q189)</f>
-        <v>551855.7646915738</v>
+        <v>557016.70284619078</v>
       </c>
       <c r="R190" s="310">
         <f t="shared" ref="R190:S190" si="73">SUM(R188:R189)</f>
-        <v>467722.19099999999</v>
+        <v>488405.07299999997</v>
       </c>
       <c r="S190" s="310">
         <f t="shared" si="73"/>
-        <v>473111.14724279998</v>
+        <v>484348.99531687499</v>
       </c>
       <c r="T190" s="310">
         <f>SUM(T188:T189)</f>
@@ -20300,15 +20421,15 @@
       </c>
       <c r="Q196" s="94">
         <f t="shared" si="74"/>
-        <v>523.19705864467312</v>
+        <v>587.70878557738467</v>
       </c>
       <c r="R196" s="94">
         <f t="shared" si="74"/>
-        <v>-2748.057585</v>
+        <v>-1403.670255</v>
       </c>
       <c r="S196" s="94">
         <f t="shared" si="74"/>
-        <v>-2397.7754292180011</v>
+        <v>-1667.3153044031251</v>
       </c>
       <c r="T196" s="94">
         <f t="shared" si="74"/>
@@ -20339,15 +20460,15 @@
       </c>
       <c r="Q197" s="90">
         <f>SUM(Q193:Q196)</f>
-        <v>38023.19705864467</v>
+        <v>38087.708785577386</v>
       </c>
       <c r="R197" s="90">
         <f>SUM(R193:R196)</f>
-        <v>34751.942414999998</v>
+        <v>36096.329745000003</v>
       </c>
       <c r="S197" s="90">
         <f>SUM(S193:S196)</f>
-        <v>35102.224570781997</v>
+        <v>35832.684695596872</v>
       </c>
       <c r="T197" s="90">
         <f>SUM(T193:T196)</f>
@@ -20378,15 +20499,15 @@
       </c>
       <c r="Q198" s="95">
         <f>IF(Q197&gt;0,Q197*(0.124+0.15+0.04),0)</f>
-        <v>11939.283876414427</v>
+        <v>11959.540558671299</v>
       </c>
       <c r="R198" s="95">
         <f>IF(R197&gt;0,R197*(0.124+0.15+0.04),0)</f>
-        <v>10912.10991831</v>
+        <v>11334.24753993</v>
       </c>
       <c r="S198" s="95">
         <f>IF(S197&gt;0,S197*(0.124+0.15+0.04),0)</f>
-        <v>11022.098515225547</v>
+        <v>11251.462994417418</v>
       </c>
       <c r="T198" s="95">
         <f>IF(T197&gt;0,T197*(0.124+0.15+0.04),0)</f>
@@ -20417,15 +20538,15 @@
       </c>
       <c r="Q199" s="97">
         <f t="shared" si="77"/>
-        <v>26083.913182230244</v>
+        <v>26128.168226906088</v>
       </c>
       <c r="R199" s="97">
         <f t="shared" si="77"/>
-        <v>23839.832496689996</v>
+        <v>24762.082205070001</v>
       </c>
       <c r="S199" s="97">
         <f t="shared" si="77"/>
-        <v>24080.126055556451</v>
+        <v>24581.221701179456</v>
       </c>
       <c r="T199" s="97">
         <f t="shared" si="77"/>
@@ -20550,15 +20671,15 @@
       </c>
       <c r="Q203" s="430">
         <f>Q189+Q199-Q200</f>
-        <v>67939.677873804088</v>
+        <v>73144.87107309686</v>
       </c>
       <c r="R203" s="430">
         <f>R189+R199-R200</f>
-        <v>-18437.976503310005</v>
+        <v>3167.1552050700011</v>
       </c>
       <c r="S203" s="430">
         <f>S189+S199-S200</f>
-        <v>-12808.726701643565</v>
+        <v>-1069.7829819455437</v>
       </c>
       <c r="T203" s="430">
         <f>T189+T199-T200</f>
@@ -20589,15 +20710,15 @@
       </c>
       <c r="Q204" s="310">
         <f t="shared" si="80"/>
-        <v>577939.67787380412</v>
+        <v>583144.87107309687</v>
       </c>
       <c r="R204" s="310">
         <f t="shared" si="80"/>
-        <v>491562.02349668997</v>
+        <v>513167.15520506998</v>
       </c>
       <c r="S204" s="310">
         <f t="shared" si="80"/>
-        <v>497191.27329835645</v>
+        <v>508930.21701805445</v>
       </c>
       <c r="T204" s="310">
         <f t="shared" si="80"/>
@@ -20784,15 +20905,15 @@
       </c>
       <c r="Q210" s="94">
         <f>IF(Q203&gt;0,Q203*$I$16,Q203*$I$15)</f>
-        <v>849.24597342255117</v>
+        <v>914.31088841371081</v>
       </c>
       <c r="R210" s="94">
         <f>IF(R203&gt;0,R203*$I$16,R203*$I$15)</f>
-        <v>-1198.4684727151503</v>
+        <v>39.589440063375015</v>
       </c>
       <c r="S210" s="94">
         <f>IF(S203&gt;0,S203*$I$16,S203*$I$15)</f>
-        <v>-832.56723560683179</v>
+        <v>-69.535893826460338</v>
       </c>
       <c r="T210" s="94">
         <f>IF(T203&gt;0,T203*$I$16,T203*$I$15)</f>
@@ -20823,15 +20944,15 @@
       </c>
       <c r="Q211" s="90">
         <f>SUM(Q207:Q210)</f>
-        <v>38349.245973422549</v>
+        <v>38414.310888413711</v>
       </c>
       <c r="R211" s="90">
         <f>SUM(R207:R210)</f>
-        <v>36301.531527284853</v>
+        <v>37539.589440063377</v>
       </c>
       <c r="S211" s="90">
         <f>SUM(S207:S210)</f>
-        <v>36667.432764393168</v>
+        <v>37430.464106173538</v>
       </c>
       <c r="T211" s="90">
         <f>SUM(T207:T210)</f>
@@ -20862,15 +20983,15 @@
       </c>
       <c r="Q212" s="95">
         <f>IF(Q211&gt;0,Q211*(0.124+0.15+0.04),0)</f>
-        <v>12041.66323565468</v>
+        <v>12062.093618961906</v>
       </c>
       <c r="R212" s="95">
         <f>IF(R211&gt;0,R211*(0.124+0.15+0.04),0)</f>
-        <v>11398.680899567444</v>
+        <v>11787.4310841799</v>
       </c>
       <c r="S212" s="95">
         <f>IF(S211&gt;0,S211*(0.124+0.15+0.04),0)</f>
-        <v>11513.573888019455</v>
+        <v>11753.165729338491</v>
       </c>
       <c r="T212" s="95">
         <f>IF(T211&gt;0,T211*(0.124+0.15+0.04),0)</f>
@@ -20901,15 +21022,15 @@
       </c>
       <c r="Q213" s="97">
         <f t="shared" si="84"/>
-        <v>26307.582737767869</v>
+        <v>26352.217269451805</v>
       </c>
       <c r="R213" s="97">
         <f t="shared" si="84"/>
-        <v>24902.850627717409</v>
+        <v>25752.158355883475</v>
       </c>
       <c r="S213" s="97">
         <f t="shared" si="84"/>
-        <v>25153.858876373713</v>
+        <v>25677.298376835046</v>
       </c>
       <c r="T213" s="97">
         <f t="shared" si="84"/>
@@ -21034,15 +21155,15 @@
       </c>
       <c r="Q217" s="430">
         <f>Q203+Q213-Q214</f>
-        <v>94247.260611571954</v>
+        <v>99497.088342548668</v>
       </c>
       <c r="R217" s="430">
         <f>R203+R213-R214</f>
-        <v>6464.8741244074045</v>
+        <v>28919.313560953477</v>
       </c>
       <c r="S217" s="430">
         <f>S203+S213-S214</f>
-        <v>12345.132174730148</v>
+        <v>24607.515394889502</v>
       </c>
       <c r="T217" s="430">
         <f>T203+T213-T214</f>
@@ -21073,15 +21194,15 @@
       </c>
       <c r="Q218" s="310">
         <f t="shared" si="87"/>
-        <v>604247.26061157195</v>
+        <v>609497.0883425487</v>
       </c>
       <c r="R218" s="310">
         <f t="shared" si="87"/>
-        <v>516464.87412440742</v>
+        <v>538919.31356095348</v>
       </c>
       <c r="S218" s="310">
         <f t="shared" si="87"/>
-        <v>522345.13217473013</v>
+        <v>534607.51539488952</v>
       </c>
       <c r="T218" s="310">
         <f t="shared" si="87"/>
@@ -21268,15 +21389,15 @@
       </c>
       <c r="Q224" s="94">
         <f>IF(Q217&gt;0,Q217*$I$16,Q217*$I$15)</f>
-        <v>1178.0907576446496</v>
+        <v>1243.7136042818584</v>
       </c>
       <c r="R224" s="94">
         <f>IF(R217&gt;0,R217*$I$16,R217*$I$15)</f>
-        <v>80.810926555092564</v>
+        <v>361.49141951191848</v>
       </c>
       <c r="S224" s="94">
         <f>IF(S217&gt;0,S217*$I$16,S217*$I$15)</f>
-        <v>154.31415218412687</v>
+        <v>307.59394243611882</v>
       </c>
       <c r="T224" s="94">
         <f>IF(T217&gt;0,T217*$I$16,T217*$I$15)</f>
@@ -21307,15 +21428,15 @@
       </c>
       <c r="Q225" s="90">
         <f>SUM(Q221:Q224)</f>
-        <v>38678.090757644648</v>
+        <v>38743.71360428186</v>
       </c>
       <c r="R225" s="90">
         <f>SUM(R221:R224)</f>
-        <v>37580.810926555096</v>
+        <v>37861.49141951192</v>
       </c>
       <c r="S225" s="90">
         <f>SUM(S221:S224)</f>
-        <v>37654.314152184124</v>
+        <v>37807.59394243612</v>
       </c>
       <c r="T225" s="90">
         <f>SUM(T221:T224)</f>
@@ -21346,15 +21467,15 @@
       </c>
       <c r="Q226" s="95">
         <f>IF(Q225&gt;0,Q225*(0.124+0.15+0.04),0)</f>
-        <v>12144.920497900419</v>
+        <v>12165.526071744503</v>
       </c>
       <c r="R226" s="95">
         <f>IF(R225&gt;0,R225*(0.124+0.15+0.04),0)</f>
-        <v>11800.3746309383</v>
+        <v>11888.508305726742</v>
       </c>
       <c r="S226" s="95">
         <f>IF(S225&gt;0,S225*(0.124+0.15+0.04),0)</f>
-        <v>11823.454643785815</v>
+        <v>11871.584497924941</v>
       </c>
       <c r="T226" s="95">
         <f>IF(T225&gt;0,T225*(0.124+0.15+0.04),0)</f>
@@ -21385,15 +21506,15 @@
       </c>
       <c r="Q227" s="97">
         <f t="shared" si="91"/>
-        <v>26533.170259744227</v>
+        <v>26578.187532537355</v>
       </c>
       <c r="R227" s="97">
         <f t="shared" si="91"/>
-        <v>25780.436295616797</v>
+        <v>25972.98311378518</v>
       </c>
       <c r="S227" s="97">
         <f t="shared" si="91"/>
-        <v>25830.859508398309</v>
+        <v>25936.009444511179</v>
       </c>
       <c r="T227" s="97">
         <f t="shared" si="91"/>
@@ -21518,15 +21639,15 @@
       </c>
       <c r="Q231" s="430">
         <f>Q217+Q227-Q228</f>
-        <v>120780.43087131617</v>
+        <v>126075.27587508602</v>
       </c>
       <c r="R231" s="430">
         <f>R217+R227-R228</f>
-        <v>32245.310420024201</v>
+        <v>54892.296674738653</v>
       </c>
       <c r="S231" s="430">
         <f>S217+S227-S228</f>
-        <v>38175.991683128457</v>
+        <v>50543.524839400678</v>
       </c>
       <c r="T231" s="430">
         <f>T217+T227-T228</f>
@@ -21557,15 +21678,15 @@
       </c>
       <c r="Q232" s="310">
         <f t="shared" ref="Q232:U232" si="94">SUM(Q230:Q231)</f>
-        <v>630780.43087131623</v>
+        <v>636075.27587508596</v>
       </c>
       <c r="R232" s="310">
         <f t="shared" si="94"/>
-        <v>542245.31042002421</v>
+        <v>564892.29667473864</v>
       </c>
       <c r="S232" s="310">
         <f t="shared" si="94"/>
-        <v>548175.99168312841</v>
+        <v>560543.52483940066</v>
       </c>
       <c r="T232" s="310">
         <f t="shared" si="94"/>
@@ -21636,15 +21757,15 @@
       </c>
       <c r="Q235" s="322">
         <f t="shared" si="95"/>
-        <v>116092.93087131623</v>
+        <v>121387.77587508596</v>
       </c>
       <c r="R235" s="322">
         <f t="shared" si="95"/>
-        <v>27557.810420024209</v>
+        <v>50204.796674738638</v>
       </c>
       <c r="S235" s="322">
         <f t="shared" si="95"/>
-        <v>33488.491683128406</v>
+        <v>45856.024839400663</v>
       </c>
       <c r="T235" s="322">
         <f t="shared" si="95"/>
@@ -21675,15 +21796,15 @@
       </c>
       <c r="Q236" s="320">
         <f t="shared" si="96"/>
-        <v>193.48821811886037</v>
+        <v>202.31295979180993</v>
       </c>
       <c r="R236" s="320">
         <f t="shared" si="96"/>
-        <v>45.929684033373682</v>
+        <v>83.674661124564395</v>
       </c>
       <c r="S236" s="320">
         <f t="shared" si="96"/>
-        <v>55.814152805214007</v>
+        <v>76.426708065667768</v>
       </c>
       <c r="T236" s="320">
         <f t="shared" si="96"/>

</xml_diff>

<commit_message>
Added functions to calculate changes in costs and revenues for Option 3: sell pairs and replace. Needs more work to match up with excel model.
</commit_message>
<xml_diff>
--- a/misc/One_Drought_User_Interface_w_NOAA_Index.xlsx
+++ b/misc/One_Drought_User_Interface_w_NOAA_Index.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="460" windowWidth="31260" windowHeight="23060" tabRatio="653" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="21580" yWindow="1100" windowWidth="31260" windowHeight="23060" tabRatio="653" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="senseInfo" sheetId="12" state="hidden" r:id="rId1"/>
@@ -13292,8 +13292,8 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AM236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="158" zoomScaleNormal="158" zoomScalePageLayoutView="158" workbookViewId="0">
-      <selection activeCell="U59" sqref="U59"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="158" zoomScaleNormal="158" zoomScalePageLayoutView="158" workbookViewId="0">
+      <selection activeCell="T166" sqref="T166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15070,8 +15070,8 @@
       <c r="AA52" s="126"/>
       <c r="AB52" s="114"/>
       <c r="AC52" s="124">
-        <f>AC51*AB16*(I16/360)</f>
-        <v>3187.5</v>
+        <f>AC51*AB16*(I16/365)</f>
+        <v>3143.8356164383567</v>
       </c>
     </row>
     <row r="53" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15102,7 +15102,7 @@
       <c r="AB53" s="114"/>
       <c r="AC53" s="124">
         <f>(AC51+AC52)*I16</f>
-        <v>6414.84375</v>
+        <v>6414.2979452054797</v>
       </c>
     </row>
     <row r="54" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15136,7 +15136,7 @@
       <c r="AB54" s="116"/>
       <c r="AC54" s="128">
         <f>(AC51+AC52+AC53)*I16</f>
-        <v>6495.029296875</v>
+        <v>6494.4766695205481</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -15351,11 +15351,11 @@
       <c r="S59" s="139"/>
       <c r="T59" s="25">
         <f>U59/I8</f>
-        <v>-5.3125</v>
+        <v>-5.2397260273972615</v>
       </c>
       <c r="U59" s="247">
-        <f>-(AC49*AB16*(I16/360))</f>
-        <v>-3187.5</v>
+        <f>-(AC49*AB16*(I16/365))</f>
+        <v>-3143.8356164383567</v>
       </c>
       <c r="W59" s="13"/>
       <c r="X59" s="149">
@@ -15405,11 +15405,11 @@
       <c r="S60" s="140"/>
       <c r="T60" s="141">
         <f>SUM(T56:T59)</f>
-        <v>193.0625</v>
+        <v>193.13527397260273</v>
       </c>
       <c r="U60" s="248">
         <f>SUM(U56:U59)</f>
-        <v>115837.5</v>
+        <v>115881.16438356164</v>
       </c>
       <c r="W60" s="13"/>
       <c r="X60" s="149">
@@ -15513,11 +15513,11 @@
       <c r="S62" s="23"/>
       <c r="T62" s="24">
         <f>U62/I8</f>
-        <v>-26.828955078124999</v>
+        <v>-26.754350385273973</v>
       </c>
       <c r="U62" s="246">
         <f>-(AC52+AC53+AC54)</f>
-        <v>-16097.373046875</v>
+        <v>-16052.610231164384</v>
       </c>
       <c r="W62" s="13"/>
       <c r="X62" s="149">
@@ -15648,11 +15648,11 @@
       <c r="S66" s="23"/>
       <c r="T66" s="24">
         <f>SUM(T61:T65)</f>
-        <v>136.08771158854165</v>
+        <v>136.16231628139269</v>
       </c>
       <c r="U66" s="246">
         <f>SUM(U61:U65)</f>
-        <v>81652.626953125</v>
+        <v>81697.389768835623</v>
       </c>
       <c r="W66" s="13"/>
     </row>
@@ -15675,11 +15675,11 @@
       <c r="S67" s="142"/>
       <c r="T67" s="143">
         <f>T60+T66</f>
-        <v>329.15021158854165</v>
+        <v>329.29759025399539</v>
       </c>
       <c r="U67" s="249">
         <f>U60+U66</f>
-        <v>197490.126953125</v>
+        <v>197578.55415239726</v>
       </c>
       <c r="W67" s="13"/>
     </row>

</xml_diff>